<commit_message>
last modified in tables
</commit_message>
<xml_diff>
--- a/public/api_info.xlsx
+++ b/public/api_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaree\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B92D419F-278A-4D10-9C5A-C63D8F226029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E9C1A3-C4C1-43EA-917D-E1BE3E9908D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{016D1DA2-1AB2-44E6-B5AB-B74B40358560}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>API_name</t>
   </si>
@@ -139,13 +139,19 @@
   </si>
   <si>
     <t>Device management</t>
+  </si>
+  <si>
+    <t>Last modified by</t>
+  </si>
+  <si>
+    <t>Last modified date &amp; time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +202,11 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="__Inter_aaf875"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,7 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -230,6 +241,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -545,22 +557,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C631B965-DEDB-4715-A324-44DAE690825C}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="30.77734375" customWidth="1"/>
     <col min="2" max="2" width="38.88671875" customWidth="1"/>
     <col min="3" max="3" width="67.5546875" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -576,8 +590,14 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -594,7 +614,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -611,7 +631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -628,7 +648,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16.8">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
@@ -645,7 +665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -662,7 +682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
@@ -679,7 +699,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
@@ -696,7 +716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update edit in carrier info and api info
</commit_message>
<xml_diff>
--- a/public/api_info.xlsx
+++ b/public/api_info.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaree\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352F7290-E038-4CC4-A826-71FA0160CA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{016D1DA2-1AB2-44E6-B5AB-B74B40358560}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,16 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
-  <si>
-    <t>API_name</t>
-  </si>
-  <si>
-    <t>API_url</t>
-  </si>
-  <si>
-    <t>API_params</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>API_state</t>
   </si>
@@ -111,9 +108,6 @@
     <t>delete,edit</t>
   </si>
   <si>
-    <t>Module_name</t>
-  </si>
-  <si>
     <t>SIM management</t>
   </si>
   <si>
@@ -183,38 +177,23 @@
     <t>25/06/2024 09:45AM</t>
   </si>
   <si>
-    <t>Success Rate</t>
-  </si>
-  <si>
-    <t>90/100</t>
-  </si>
-  <si>
-    <t>70/100</t>
-  </si>
-  <si>
-    <t>20/100</t>
-  </si>
-  <si>
-    <t>50/100</t>
-  </si>
-  <si>
-    <t>30/100</t>
-  </si>
-  <si>
-    <t>43/100</t>
-  </si>
-  <si>
-    <t>33/100</t>
-  </si>
-  <si>
-    <t>Last sync date &amp; time</t>
+    <t>API name</t>
+  </si>
+  <si>
+    <t>API url</t>
+  </si>
+  <si>
+    <t>API params</t>
+  </si>
+  <si>
+    <t>Module name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,7 +339,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -412,7 +391,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -606,276 +585,224 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C631B965-DEDB-4715-A324-44DAE690825C}">
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="67.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.77734375" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="67.5546875" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="25.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" t="s">
-        <v>51</v>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" t="s">
-        <v>52</v>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
         <v>44</v>
       </c>
-      <c r="I3" t="s">
-        <v>53</v>
-      </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" t="s">
-        <v>54</v>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16.5">
-      <c r="A5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="C6" r:id="rId3"/>
-    <hyperlink ref="C7" r:id="rId4"/>
-    <hyperlink ref="C3" r:id="rId5"/>
-    <hyperlink ref="C4" r:id="rId6"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{B44482FA-D716-4D49-BE93-5DE1F7C1AC0C}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{C2FA5BBB-23C5-4BC4-AF9A-78DBDD58F03B}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{70A30663-97C1-455A-BE4F-CF329E36ED5E}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{7DF2C81F-50AC-46A7-AD4C-FDF72F810780}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{3588E65B-FCE0-4004-968B-F297F08C8DBA}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{A9F111B5-9EF2-469C-9D81-E0E3422E5BC4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>